<commit_message>
Update to compatibility matrix
</commit_message>
<xml_diff>
--- a/logs/compatibility_matrix.xlsx
+++ b/logs/compatibility_matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\HiwiJob\PredMSiamNN\logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niklas\Dropbox\HiwiJob\PredMSiamNN\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6FFE5B-A359-468A-8F65-C3E51E63EFEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE983844-7075-44A7-9DD6-1D7A7D534611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Encoder</t>
   </si>
@@ -84,18 +84,12 @@
     <t>Descriptions:</t>
   </si>
   <si>
-    <t>Features for additional inputs not implemented yet.</t>
-  </si>
-  <si>
     <t>Working</t>
   </si>
   <si>
     <t>Not working / errors when executing</t>
   </si>
   <si>
-    <t>Shall/can not work or planned feature</t>
-  </si>
-  <si>
     <t>Unclear / not yet tested</t>
   </si>
   <si>
@@ -106,6 +100,15 @@
   </si>
   <si>
     <t>Not working due to *1</t>
+  </si>
+  <si>
+    <t>Can not work or planned feature</t>
+  </si>
+  <si>
+    <t>Not planned / necessary</t>
+  </si>
+  <si>
+    <t>Additional input not necessary for CBS, it would be [1, 1, …., 1]</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +188,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -262,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -278,7 +287,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -291,6 +299,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -573,45 +583,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.5703125" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="17" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="19"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -686,19 +696,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -708,10 +714,10 @@
       <c r="C8" s="12"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -725,13 +731,13 @@
         <v>13</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
@@ -747,22 +753,27 @@
     </row>
     <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="19" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -791,20 +802,20 @@
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>